<commit_message>
Documentación y SCRIPTS para ambiente de Pruebas ASN_PE
</commit_message>
<xml_diff>
--- a/Documentos/Planes de Trabajo/Plan de Trabajo Multi-seleccion de Clientes en Perfil de Empleados v3.xlsx
+++ b/Documentos/Planes de Trabajo/Plan de Trabajo Multi-seleccion de Clientes en Perfil de Empleados v3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t xml:space="preserve">Semana 0</t>
   </si>
@@ -515,9 +515,9 @@
   <dimension ref="B1:BA28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="8765" ySplit="0" topLeftCell="AA1" activePane="topRight" state="split"/>
+      <pane xSplit="8103" ySplit="0" topLeftCell="A1" activePane="topLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AA14" activeCellId="0" sqref="14:14"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1388,7 +1388,7 @@
       <c r="BA11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="15" t="n">
+      <c r="B12" s="14" t="n">
         <v>8</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1453,7 +1453,7 @@
       <c r="BA12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15" t="n">
+      <c r="B13" s="14" t="n">
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -1509,10 +1509,10 @@
       <c r="BA13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15" t="n">
+      <c r="B14" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="15"/>
@@ -1546,7 +1546,9 @@
       <c r="AA14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="AB14" s="23"/>
+      <c r="AB14" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="AC14" s="17"/>
       <c r="AD14" s="17"/>
       <c r="AE14" s="24"/>
@@ -1592,7 +1594,7 @@
       <c r="AD15" s="27"/>
       <c r="AE15" s="24"/>
       <c r="AF15" s="24"/>
-      <c r="AG15" s="20"/>
+      <c r="AG15" s="27"/>
       <c r="AH15" s="20"/>
       <c r="AL15" s="24"/>
       <c r="AM15" s="24"/>
@@ -1631,8 +1633,7 @@
       <c r="X16" s="24"/>
       <c r="Y16" s="24"/>
       <c r="AA16" s="17"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="17"/>
+      <c r="AC16" s="23"/>
       <c r="AD16" s="17"/>
       <c r="AE16" s="24"/>
       <c r="AF16" s="24"/>

</xml_diff>